<commit_message>
DB events task updated
Sprint 2
</commit_message>
<xml_diff>
--- a/Sprint1_UserStories.xlsx.xlsx
+++ b/Sprint1_UserStories.xlsx.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
   <si>
     <t>User Story</t>
   </si>
@@ -797,6 +797,54 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6350000" cy="6350000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -7317,7 +7365,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -7411,7 +7459,9 @@
         <v>41</v>
       </c>
       <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
+      <c r="D6" s="21" t="s">
+        <v>20</v>
+      </c>
       <c r="E6" s="21"/>
       <c r="F6" s="21"/>
     </row>

</xml_diff>

<commit_message>
Completed initial design for ios application and updated user story sheet.
</commit_message>
<xml_diff>
--- a/Sprint1_UserStories.xlsx.xlsx
+++ b/Sprint1_UserStories.xlsx.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="46">
   <si>
     <t>User Story</t>
   </si>
@@ -350,15 +350,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -894,6 +894,62 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>228600</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="AutoShape 1"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="6350000" cy="6350000"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="r" b="b"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rtlCol="0"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1518,35 +1574,35 @@
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15"/>
-      <c r="B25" s="16" t="s">
+      <c r="B25" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="17"/>
-      <c r="D25" s="17"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="17"/>
-      <c r="D26" s="17"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="17"/>
-      <c r="D27" s="17"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="17"/>
-      <c r="D28" s="17"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
+      <c r="B29" s="20"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15"/>
@@ -7414,7 +7470,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7427,178 +7483,182 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="C1" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="18" t="s">
+      <c r="D1" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="20">
+      <c r="A2" s="18">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20" t="s">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="20">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="18"/>
+      <c r="D3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
     </row>
     <row r="4" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="20">
+      <c r="A4" s="18">
         <v>3</v>
       </c>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20" t="s">
+      <c r="C4" s="18"/>
+      <c r="D4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="E4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="18"/>
     </row>
     <row r="5" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="20">
+      <c r="A5" s="18">
         <v>4</v>
       </c>
-      <c r="B5" s="20" t="s">
+      <c r="B5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20" t="s">
+      <c r="C5" s="18"/>
+      <c r="D5" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
+      <c r="E5" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="20">
+      <c r="A6" s="18">
         <v>5</v>
       </c>
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
     </row>
     <row r="7" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="20">
+      <c r="A7" s="18">
         <v>6</v>
       </c>
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20" t="s">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="18"/>
     </row>
     <row r="8" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="20">
+      <c r="A8" s="18">
         <v>7</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="18"/>
+      <c r="D8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="18"/>
     </row>
     <row r="9" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="20">
+      <c r="A9" s="18">
         <v>8</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20" t="s">
+      <c r="C9" s="18"/>
+      <c r="D9" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
     </row>
     <row r="10" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
+      <c r="A10" s="18">
         <v>9</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20" t="s">
+      <c r="C10" s="18"/>
+      <c r="D10" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
     </row>
     <row r="11" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="20">
+      <c r="A11" s="18">
         <v>10</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="18" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20" t="s">
+      <c r="C11" s="18"/>
+      <c r="D11" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="E11" s="18"/>
+      <c r="F11" s="18"/>
     </row>
     <row r="12" spans="1:6" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="20">
+      <c r="A12" s="18">
         <v>11</v>
       </c>
-      <c r="B12" s="20" t="s">
+      <c r="B12" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20" t="s">
+      <c r="C12" s="18"/>
+      <c r="D12" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>